<commit_message>
Lodging people to households.
</commit_message>
<xml_diff>
--- a/data/processed/poland/DW/production_age.xlsx
+++ b/data/processed/poland/DW/production_age.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="36">
   <si>
     <t xml:space="preserve">age</t>
   </si>
@@ -31,12 +31,18 @@
     <t xml:space="preserve">economic_group</t>
   </si>
   <si>
+    <t xml:space="preserve">generation</t>
+  </si>
+  <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">preproduction</t>
   </si>
   <si>
+    <t xml:space="preserve">young</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
@@ -82,6 +88,9 @@
     <t xml:space="preserve">30-34</t>
   </si>
   <si>
+    <t xml:space="preserve">middle</t>
+  </si>
+  <si>
     <t xml:space="preserve">35-39</t>
   </si>
   <si>
@@ -98,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">60-64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elderly</t>
   </si>
   <si>
     <t xml:space="preserve">65-69</t>
@@ -238,10 +250,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44:D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -259,159 +271,204 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -422,7 +479,10 @@
         <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,7 +493,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +507,10 @@
         <v>0</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +521,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,7 +535,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,7 +549,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +563,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,7 +577,10 @@
         <v>0</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +591,10 @@
         <v>0</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,7 +605,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +619,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +633,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +647,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,7 +661,10 @@
         <v>0</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,7 +675,10 @@
         <v>0</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,293 +689,374 @@
         <v>0</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>27</v>
+      <c r="D43" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,7 +1067,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,7 +1081,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,7 +1095,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -917,7 +1109,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,7 +1123,10 @@
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,7 +1137,10 @@
         <v>1</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +1151,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,7 +1165,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,7 +1179,10 @@
         <v>1</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,7 +1193,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1207,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +1221,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1235,10 @@
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,7 +1249,10 @@
         <v>1</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1263,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,139 +1277,178 @@
         <v>1</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B77" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D83" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B83" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B85" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>27</v>
+      <c r="D85" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>